<commit_message>
Generate docs now sorts so 'required' props are first, and generates .full.json for each entity An attempt to solidify CT core DM - added requirement for "common" fields json_validator now forces absent additional keys for any '$ref' node which is compliant with json-schema: "You will always use $ref as the only key in an object: any other keys you put there will be ignored by the validator." renaming / moving some sample/aliquot fields docs improved for properties with 'allOf->$refs` template_writer now uses proper '$comment' field for comments WES output - with somatic var call wes_output refactor after Priti review fixed CT examples for test_clinicaltrial_examples sample status -> aliquot status, etc renaming Prism rework for json pointers instead of grep and hints prism for wes embeded in a new way .csv's for all template_examples updated new prism way - check wes_template.json
</commit_message>
<xml_diff>
--- a/template_examples/analyte_template.xlsx
+++ b/template_examples/analyte_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B17871B-D69E-2B46-B973-08A1F06F751F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B82A05-83B4-BC44-859C-8EC0050282C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2700" yWindow="-19360" windowWidth="26800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tissue" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -511,7 +511,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -524,7 +524,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -537,7 +537,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -563,7 +563,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -701,9 +701,6 @@
     <t>EXTRACTED UNITS</t>
   </si>
   <si>
-    <t>SAMPLE AMOUNT</t>
-  </si>
-  <si>
     <t>CIMAC ALIQUOT ID</t>
   </si>
   <si>
@@ -713,15 +710,6 @@
     <t>MATERIAL REMAINING</t>
   </si>
   <si>
-    <t>SAMPLE QUALITY STATUS</t>
-  </si>
-  <si>
-    <t>SAMPLE REPLACEMENT</t>
-  </si>
-  <si>
-    <t>SAMPLE STATUS</t>
-  </si>
-  <si>
     <t>R123</t>
   </si>
   <si>
@@ -782,20 +770,32 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Sample Leftover</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>ALIQUOT STATUS</t>
+  </si>
+  <si>
+    <t>Aliquot Leftover</t>
+  </si>
+  <si>
+    <t>ALIQUOT REPLACEMENT</t>
+  </si>
+  <si>
+    <t>ALIQUOT AMOUNT</t>
+  </si>
+  <si>
+    <t>ALIQUOT QUALITY STATUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +814,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -890,13 +896,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:Y28"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1251,32 +1257,32 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
     </row>
     <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1352,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1385,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1418,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1550,7 +1556,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1583,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1616,7 +1622,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1649,7 +1655,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1681,7 +1687,7 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1814,7 +1820,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1847,7 +1853,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1873,34 +1879,34 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1958,25 +1964,25 @@
         <v>40</v>
       </c>
       <c r="S22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V22" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -2004,38 +2010,38 @@
       <c r="H23">
         <v>12345</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" t="s">
         <v>57</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" t="s">
-        <v>59</v>
-      </c>
-      <c r="L23" t="s">
-        <v>60</v>
-      </c>
-      <c r="M23" t="s">
-        <v>61</v>
       </c>
       <c r="N23">
         <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q23">
         <v>134</v>
       </c>
       <c r="R23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T23">
         <v>12344</v>
@@ -2047,13 +2053,13 @@
         <v>100</v>
       </c>
       <c r="W23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X23" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y23" t="s">
         <v>67</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -2081,38 +2087,38 @@
       <c r="H24">
         <v>12345</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" t="s">
         <v>57</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" t="s">
-        <v>60</v>
-      </c>
-      <c r="M24" t="s">
-        <v>61</v>
       </c>
       <c r="N24">
         <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q24">
         <v>123</v>
       </c>
       <c r="R24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T24">
         <v>12344</v>
@@ -2124,13 +2130,13 @@
         <v>100</v>
       </c>
       <c r="W24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X24" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y24" t="s">
         <v>67</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2158,38 +2164,38 @@
       <c r="H25">
         <v>12345</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" t="s">
         <v>57</v>
-      </c>
-      <c r="J25" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L25" t="s">
-        <v>60</v>
-      </c>
-      <c r="M25" t="s">
-        <v>61</v>
       </c>
       <c r="N25">
         <v>10</v>
       </c>
       <c r="O25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q25">
         <v>43</v>
       </c>
       <c r="R25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T25">
         <v>12344</v>
@@ -2201,13 +2207,13 @@
         <v>100</v>
       </c>
       <c r="W25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X25" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y25" t="s">
         <v>67</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2235,38 +2241,38 @@
       <c r="H26">
         <v>12345</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" t="s">
         <v>57</v>
-      </c>
-      <c r="J26" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" t="s">
-        <v>59</v>
-      </c>
-      <c r="L26" t="s">
-        <v>60</v>
-      </c>
-      <c r="M26" t="s">
-        <v>61</v>
       </c>
       <c r="N26">
         <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q26">
         <v>64</v>
       </c>
       <c r="R26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T26">
         <v>12344</v>
@@ -2278,13 +2284,13 @@
         <v>100</v>
       </c>
       <c r="W26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X26" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y26" t="s">
         <v>67</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -2312,38 +2318,38 @@
       <c r="H27">
         <v>12345</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" t="s">
         <v>57</v>
-      </c>
-      <c r="J27" t="s">
-        <v>69</v>
-      </c>
-      <c r="K27" t="s">
-        <v>59</v>
-      </c>
-      <c r="L27" t="s">
-        <v>60</v>
-      </c>
-      <c r="M27" t="s">
-        <v>61</v>
       </c>
       <c r="N27">
         <v>10</v>
       </c>
       <c r="O27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q27">
         <v>23</v>
       </c>
       <c r="R27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T27">
         <v>12344</v>
@@ -2355,13 +2361,13 @@
         <v>100</v>
       </c>
       <c r="W27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X27" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y27" t="s">
         <v>67</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2389,38 +2395,38 @@
       <c r="H28">
         <v>12345</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" t="s">
         <v>57</v>
-      </c>
-      <c r="J28" t="s">
-        <v>70</v>
-      </c>
-      <c r="K28" t="s">
-        <v>59</v>
-      </c>
-      <c r="L28" t="s">
-        <v>60</v>
-      </c>
-      <c r="M28" t="s">
-        <v>61</v>
       </c>
       <c r="N28">
         <v>10</v>
       </c>
       <c r="O28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q28">
         <v>53</v>
       </c>
       <c r="R28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T28">
         <v>12344</v>
@@ -2432,13 +2438,13 @@
         <v>100</v>
       </c>
       <c r="W28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y28" t="s">
         <v>67</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -3417,7 +3423,7 @@
     <mergeCell ref="B21:S21"/>
     <mergeCell ref="T21:Y21"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{0452EA3B-E92B-4B48-9BFF-D3067ED8E573}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
@@ -3451,11 +3457,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X23:X222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y29:Y222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y28" xr:uid="{FC4C52AC-F5DB-BE49-BB0E-2EABBB22246D}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{374FBEED-5C81-484F-844C-8A7842810AA7}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sample status -> aliquot status, etc renaming
</commit_message>
<xml_diff>
--- a/template_examples/analyte_template.xlsx
+++ b/template_examples/analyte_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B17871B-D69E-2B46-B973-08A1F06F751F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13B82A05-83B4-BC44-859C-8EC0050282C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2700" yWindow="-19360" windowWidth="26800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tissue" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -511,7 +511,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -524,7 +524,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -537,7 +537,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -563,7 +563,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -701,9 +701,6 @@
     <t>EXTRACTED UNITS</t>
   </si>
   <si>
-    <t>SAMPLE AMOUNT</t>
-  </si>
-  <si>
     <t>CIMAC ALIQUOT ID</t>
   </si>
   <si>
@@ -713,15 +710,6 @@
     <t>MATERIAL REMAINING</t>
   </si>
   <si>
-    <t>SAMPLE QUALITY STATUS</t>
-  </si>
-  <si>
-    <t>SAMPLE REPLACEMENT</t>
-  </si>
-  <si>
-    <t>SAMPLE STATUS</t>
-  </si>
-  <si>
     <t>R123</t>
   </si>
   <si>
@@ -782,20 +770,32 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Sample Leftover</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>ALIQUOT STATUS</t>
+  </si>
+  <si>
+    <t>Aliquot Leftover</t>
+  </si>
+  <si>
+    <t>ALIQUOT REPLACEMENT</t>
+  </si>
+  <si>
+    <t>ALIQUOT AMOUNT</t>
+  </si>
+  <si>
+    <t>ALIQUOT QUALITY STATUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -814,6 +814,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -890,13 +896,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:Y28"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1251,32 +1257,32 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
     </row>
     <row r="2" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1352,7 +1358,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1385,7 +1391,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1418,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -1550,7 +1556,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1583,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1616,7 +1622,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1649,7 +1655,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1681,7 +1687,7 @@
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>41590</v>
       </c>
       <c r="D14" s="1"/>
@@ -1814,7 +1820,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1847,7 +1853,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1873,34 +1879,34 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1958,25 +1964,25 @@
         <v>40</v>
       </c>
       <c r="S22" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="U22" s="2" t="s">
+      <c r="V22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="V22" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="W22" s="2" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="X22" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.2">
@@ -2004,38 +2010,38 @@
       <c r="H23">
         <v>12345</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="I23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J23" t="s">
+        <v>54</v>
+      </c>
+      <c r="K23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L23" t="s">
+        <v>56</v>
+      </c>
+      <c r="M23" t="s">
         <v>57</v>
-      </c>
-      <c r="J23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" t="s">
-        <v>59</v>
-      </c>
-      <c r="L23" t="s">
-        <v>60</v>
-      </c>
-      <c r="M23" t="s">
-        <v>61</v>
       </c>
       <c r="N23">
         <v>10</v>
       </c>
       <c r="O23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P23" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q23">
         <v>134</v>
       </c>
       <c r="R23" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T23">
         <v>12344</v>
@@ -2047,13 +2053,13 @@
         <v>100</v>
       </c>
       <c r="W23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X23" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y23" t="s">
         <v>67</v>
-      </c>
-      <c r="Y23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
@@ -2081,38 +2087,38 @@
       <c r="H24">
         <v>12345</v>
       </c>
-      <c r="I24" s="5" t="s">
+      <c r="I24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" t="s">
+        <v>56</v>
+      </c>
+      <c r="M24" t="s">
         <v>57</v>
-      </c>
-      <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" t="s">
-        <v>60</v>
-      </c>
-      <c r="M24" t="s">
-        <v>61</v>
       </c>
       <c r="N24">
         <v>10</v>
       </c>
       <c r="O24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q24">
         <v>123</v>
       </c>
       <c r="R24" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S24" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T24">
         <v>12344</v>
@@ -2124,13 +2130,13 @@
         <v>100</v>
       </c>
       <c r="W24" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X24" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y24" t="s">
         <v>67</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
@@ -2158,38 +2164,38 @@
       <c r="H25">
         <v>12345</v>
       </c>
-      <c r="I25" s="5" t="s">
+      <c r="I25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" t="s">
+        <v>65</v>
+      </c>
+      <c r="K25" t="s">
+        <v>55</v>
+      </c>
+      <c r="L25" t="s">
+        <v>56</v>
+      </c>
+      <c r="M25" t="s">
         <v>57</v>
-      </c>
-      <c r="J25" t="s">
-        <v>70</v>
-      </c>
-      <c r="K25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L25" t="s">
-        <v>60</v>
-      </c>
-      <c r="M25" t="s">
-        <v>61</v>
       </c>
       <c r="N25">
         <v>10</v>
       </c>
       <c r="O25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P25" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q25">
         <v>43</v>
       </c>
       <c r="R25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T25">
         <v>12344</v>
@@ -2201,13 +2207,13 @@
         <v>100</v>
       </c>
       <c r="W25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X25" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y25" t="s">
         <v>67</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.2">
@@ -2235,38 +2241,38 @@
       <c r="H26">
         <v>12345</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K26" t="s">
+        <v>55</v>
+      </c>
+      <c r="L26" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" t="s">
         <v>57</v>
-      </c>
-      <c r="J26" t="s">
-        <v>58</v>
-      </c>
-      <c r="K26" t="s">
-        <v>59</v>
-      </c>
-      <c r="L26" t="s">
-        <v>60</v>
-      </c>
-      <c r="M26" t="s">
-        <v>61</v>
       </c>
       <c r="N26">
         <v>10</v>
       </c>
       <c r="O26" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q26">
         <v>64</v>
       </c>
       <c r="R26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T26">
         <v>12344</v>
@@ -2278,13 +2284,13 @@
         <v>100</v>
       </c>
       <c r="W26" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X26" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y26" t="s">
         <v>67</v>
-      </c>
-      <c r="Y26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.2">
@@ -2312,38 +2318,38 @@
       <c r="H27">
         <v>12345</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="I27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" t="s">
+        <v>64</v>
+      </c>
+      <c r="K27" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" t="s">
+        <v>56</v>
+      </c>
+      <c r="M27" t="s">
         <v>57</v>
-      </c>
-      <c r="J27" t="s">
-        <v>69</v>
-      </c>
-      <c r="K27" t="s">
-        <v>59</v>
-      </c>
-      <c r="L27" t="s">
-        <v>60</v>
-      </c>
-      <c r="M27" t="s">
-        <v>61</v>
       </c>
       <c r="N27">
         <v>10</v>
       </c>
       <c r="O27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q27">
         <v>23</v>
       </c>
       <c r="R27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T27">
         <v>12344</v>
@@ -2355,13 +2361,13 @@
         <v>100</v>
       </c>
       <c r="W27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X27" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y27" t="s">
         <v>67</v>
-      </c>
-      <c r="Y27" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.2">
@@ -2389,38 +2395,38 @@
       <c r="H28">
         <v>12345</v>
       </c>
-      <c r="I28" s="5" t="s">
+      <c r="I28" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
+        <v>55</v>
+      </c>
+      <c r="L28" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" t="s">
         <v>57</v>
-      </c>
-      <c r="J28" t="s">
-        <v>70</v>
-      </c>
-      <c r="K28" t="s">
-        <v>59</v>
-      </c>
-      <c r="L28" t="s">
-        <v>60</v>
-      </c>
-      <c r="M28" t="s">
-        <v>61</v>
       </c>
       <c r="N28">
         <v>10</v>
       </c>
       <c r="O28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="P28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q28">
         <v>53</v>
       </c>
       <c r="R28" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S28" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="T28">
         <v>12344</v>
@@ -2432,13 +2438,13 @@
         <v>100</v>
       </c>
       <c r="W28" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="X28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y28" t="s">
         <v>67</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
@@ -3417,7 +3423,7 @@
     <mergeCell ref="B21:S21"/>
     <mergeCell ref="T21:Y21"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{0452EA3B-E92B-4B48-9BFF-D3067ED8E573}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
@@ -3451,11 +3457,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X23:X222" xr:uid="{00000000-0002-0000-0000-00000B000000}">
       <formula1>"Replacement Requested,Replacement Tested,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y29:Y222" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other,Sample Leftover"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y28" xr:uid="{FC4C52AC-F5DB-BE49-BB0E-2EABBB22246D}">
-      <formula1>"Sample Returned,Sample Exhausted,Remainder used for other Assay,Other"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y23:Y222" xr:uid="{374FBEED-5C81-484F-844C-8A7842810AA7}">
+      <formula1>"Aliquot Returned,Aliquot Exhausted,Remainder used for other Assay,Other,Aliquot Leftover"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>